<commit_message>
New SIS and MILS working
</commit_message>
<xml_diff>
--- a/OLS/SIS/Input and Constants/sis_in_bo.xlsx
+++ b/OLS/SIS/Input and Constants/sis_in_bo.xlsx
@@ -161,10 +161,10 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.29"/>

</xml_diff>